<commit_message>
alterei o UserStory, UX e backlog
</commit_message>
<xml_diff>
--- a/documentação/product-backlog-get-mobi.xlsx
+++ b/documentação/product-backlog-get-mobi.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/831f5f1da6d5c7f7/Documentos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bandtec\getmobi\documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AC4C3058-0581-49EB-ABBD-4DF3CD699DED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5106A842-9BC4-44E2-B7B5-6713F51A6580}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PBC" sheetId="1" r:id="rId1"/>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="65">
   <si>
     <t>Product BackLog Classified (PBC)</t>
   </si>
@@ -112,99 +112,33 @@
     <t>Em Andamento</t>
   </si>
   <si>
-    <t>US#1 Cadastro</t>
-  </si>
-  <si>
     <t>O site deve ter uma pagina de cadastro para ter acesso ao sistema</t>
   </si>
   <si>
-    <t>US#2 Login</t>
-  </si>
-  <si>
-    <t>O site deve ter uma página de login para entrar no sistema</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
-    <t>US#3 Monitorar</t>
-  </si>
-  <si>
     <t xml:space="preserve">O sistema deve monitorar o aluno que estiver interessado </t>
   </si>
   <si>
     <t>Planejada</t>
   </si>
   <si>
-    <t>US#4 Newsletter</t>
-  </si>
-  <si>
     <t xml:space="preserve">O sistema deve enviar por e-mail campanhas informativas </t>
   </si>
   <si>
     <t>o sistema deve enviar alertas para os professores sobre uso indevido</t>
   </si>
   <si>
-    <t>enviar sequencias aleatórias de palavras para o aluno</t>
-  </si>
-  <si>
-    <t>US#7 Relatório</t>
-  </si>
-  <si>
     <t>Envio para os professores de relatórios do desempenho dos alunos</t>
   </si>
   <si>
     <t>o sistema deverá tirar print da tela em um periodo estimado</t>
   </si>
   <si>
-    <t>US#9 Gráfico</t>
-  </si>
-  <si>
     <t>o sistema deverá ter um dashboard com gráficos para analise de dados</t>
   </si>
   <si>
-    <t>CC#10&lt;Localização&gt;</t>
-  </si>
-  <si>
-    <t>O sistema deverá usar API de Geo Localização</t>
-  </si>
-  <si>
-    <t>CC#10.1&lt;Localização&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O sistema deverá usar API deverá possibilitar calculo de distância entre dois pontos </t>
-  </si>
-  <si>
-    <t>CC#10.2&lt;Localização&gt;</t>
-  </si>
-  <si>
-    <t>O sistema deverá ter um Pin para demonstra a localização do Usuário</t>
-  </si>
-  <si>
-    <t>US#11&lt;&gt;</t>
-  </si>
-  <si>
-    <t>US#11.1&lt;&gt;</t>
-  </si>
-  <si>
-    <t>US#12&lt;&gt;</t>
-  </si>
-  <si>
-    <t>US#13&lt;&gt;</t>
-  </si>
-  <si>
-    <t>JU#14&lt;&gt;</t>
-  </si>
-  <si>
-    <t>BP#15&lt;&gt;</t>
-  </si>
-  <si>
-    <t>US#16&lt;&gt;</t>
-  </si>
-  <si>
-    <t>DR#17&lt;&gt;</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
@@ -298,13 +232,52 @@
     <t>EC</t>
   </si>
   <si>
-    <t xml:space="preserve">US#5 Alerta </t>
-  </si>
-  <si>
-    <t>US#6 Pop-ups</t>
-  </si>
-  <si>
-    <t>US#8 Printscreen</t>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Enviar sequencias aleatórias de palavras para o aluno</t>
+  </si>
+  <si>
+    <t>O site deve ter uma página de login</t>
+  </si>
+  <si>
+    <t>CC#1 &lt;APIs&gt;</t>
+  </si>
+  <si>
+    <t>O sistema deve ter APIs para capturar dados de maquina dos alunos</t>
+  </si>
+  <si>
+    <t>US#6 &lt;Rankings&gt;</t>
+  </si>
+  <si>
+    <t>US#4 &lt;Gráfico&gt;</t>
+  </si>
+  <si>
+    <t>US#2 &lt;Printscreen&gt;</t>
+  </si>
+  <si>
+    <t>US#4 &lt;Relatório&gt;</t>
+  </si>
+  <si>
+    <t>US#3 &lt;Pop-ups&gt;</t>
+  </si>
+  <si>
+    <t>US#2 &lt;Alerta&gt;</t>
+  </si>
+  <si>
+    <t>US#4 &lt;Newsletter&gt;</t>
+  </si>
+  <si>
+    <t>US#1 &lt;Monitorar&gt;</t>
+  </si>
+  <si>
+    <t>US#2 &lt;Login&gt;</t>
+  </si>
+  <si>
+    <t>US#1 &lt;Cadastro&gt;</t>
+  </si>
+  <si>
+    <t>O sistema deve apresentar rankings para acompanhar desempenho dos alunos</t>
   </si>
 </sst>
 </file>
@@ -523,9 +496,6 @@
   </cellStyleXfs>
   <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -655,6 +625,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -662,7 +635,73 @@
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="30">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBFBFBF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEFB661"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFC8D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBFBFBF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEFB661"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFC8D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1541,636 +1580,613 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ51"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="21"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="42.7109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="78.85546875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="0.7109375" style="4" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" style="2" customWidth="1"/>
-    <col min="9" max="10" width="8.85546875" style="2"/>
-    <col min="11" max="11" width="13.7109375" style="2" customWidth="1"/>
-    <col min="12" max="1024" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="3.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="42.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="78.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="0.7109375" style="3" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" style="1" customWidth="1"/>
+    <col min="9" max="10" width="8.85546875" style="1"/>
+    <col min="11" max="11" width="13.7109375" style="1" customWidth="1"/>
+    <col min="12" max="1024" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="19.5" customHeight="1"/>
     <row r="2" spans="2:11" ht="89.25" customHeight="1">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
     </row>
     <row r="3" spans="2:11" ht="9.9499999999999993" customHeight="1"/>
-    <row r="4" spans="2:11" s="6" customFormat="1" ht="24.95" customHeight="1">
-      <c r="B4" s="7" t="s">
+    <row r="4" spans="2:11" s="5" customFormat="1" ht="24.95" customHeight="1">
+      <c r="B4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:11" s="12" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B5" s="13" t="s">
+    <row r="5" spans="2:11" s="11" customFormat="1" ht="28.5" customHeight="1">
+      <c r="B5" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="E5" s="15"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="16"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17" t="s">
+      <c r="H5" s="16"/>
+    </row>
+    <row r="6" spans="2:11" s="11" customFormat="1" ht="23.1" customHeight="1">
+      <c r="B6" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="15"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="16"/>
+    </row>
+    <row r="7" spans="2:11" s="11" customFormat="1" ht="23.1" customHeight="1">
+      <c r="B7" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="15"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="16"/>
+    </row>
+    <row r="8" spans="2:11" s="11" customFormat="1" ht="23.1" customHeight="1">
+      <c r="B8" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="17"/>
-    </row>
-    <row r="6" spans="2:11" s="12" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B6" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="18" t="s">
+      <c r="E8" s="21"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+    </row>
+    <row r="9" spans="2:11" s="11" customFormat="1" ht="32.25" customHeight="1">
+      <c r="B9" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="16"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="17"/>
-    </row>
-    <row r="7" spans="2:11" s="12" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B7" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="19" t="s">
+      <c r="C9" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="E9" s="15"/>
+      <c r="F9" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+    </row>
+    <row r="10" spans="2:11" s="11" customFormat="1" ht="23.1" customHeight="1">
+      <c r="B10" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" s="21"/>
+      <c r="F10" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+    </row>
+    <row r="11" spans="2:11" s="11" customFormat="1" ht="33.75" customHeight="1">
+      <c r="B11" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="16"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" s="17"/>
-    </row>
-    <row r="8" spans="2:11" s="12" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B8" s="13" t="s">
+      <c r="E11" s="21"/>
+      <c r="F11" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+    </row>
+    <row r="12" spans="2:11" s="11" customFormat="1" ht="23.1" customHeight="1">
+      <c r="B12" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="E12" s="21"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" s="11" customFormat="1" ht="31.5" customHeight="1">
+      <c r="B13" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="22"/>
-      <c r="F8" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="23"/>
-    </row>
-    <row r="9" spans="2:11" s="12" customFormat="1" ht="22.5" customHeight="1">
-      <c r="B9" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="D9" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-    </row>
-    <row r="10" spans="2:11" s="12" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B10" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="D10" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="22"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11" s="12" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B11" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="22"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" s="12" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B12" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="D12" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="22"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" s="12" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B13" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="E13" s="22"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" s="12" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B14" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="22"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-    </row>
-    <row r="15" spans="2:11" s="12" customFormat="1" ht="30">
-      <c r="B15" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="E15" s="22"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="17"/>
-    </row>
-    <row r="16" spans="2:11" s="12" customFormat="1" ht="30">
-      <c r="B16" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="E16" s="22"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-    </row>
-    <row r="17" spans="2:8" s="12" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B17" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="D17" s="25"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-    </row>
-    <row r="18" spans="2:8" s="12" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B18" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" s="26"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-    </row>
-    <row r="19" spans="2:8" s="12" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B19" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" s="26"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-    </row>
-    <row r="20" spans="2:8" s="12" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B20" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="D20" s="26"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
-    </row>
-    <row r="21" spans="2:8" s="12" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B21" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21" s="26"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
-    </row>
-    <row r="22" spans="2:8" s="12" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B22" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C22" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="D22" s="26"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-    </row>
-    <row r="23" spans="2:8" s="12" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B23" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C23" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="D23" s="26"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-    </row>
-    <row r="24" spans="2:8" s="12" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B24" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="D24" s="26"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
-    </row>
-    <row r="25" spans="2:8" s="12" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B25" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C25" s="14"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="22"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="17"/>
-    </row>
-    <row r="26" spans="2:8" s="12" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B26" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C26" s="14"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="17"/>
-    </row>
-    <row r="27" spans="2:8" s="12" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B27" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C27" s="14"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="17"/>
-    </row>
-    <row r="28" spans="2:8" s="12" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B28" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C28" s="14"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="17"/>
-      <c r="H28" s="17"/>
-    </row>
-    <row r="29" spans="2:8" s="12" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B29" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C29" s="14"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="17"/>
-      <c r="H29" s="17"/>
-    </row>
-    <row r="30" spans="2:8" s="12" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B30" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C30" s="14"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="17"/>
-    </row>
-    <row r="31" spans="2:8" s="12" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B31" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C31" s="14"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="22"/>
-      <c r="F31" s="17"/>
-      <c r="G31" s="17"/>
-      <c r="H31" s="17"/>
-    </row>
-    <row r="32" spans="2:8" s="12" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B32" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C32" s="14"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="17"/>
-      <c r="G32" s="17"/>
-      <c r="H32" s="17"/>
-    </row>
-    <row r="33" spans="2:8" s="12" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B33" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C33" s="14"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="22"/>
-      <c r="F33" s="17"/>
-      <c r="G33" s="17"/>
-      <c r="H33" s="17"/>
-    </row>
-    <row r="34" spans="2:8" s="12" customFormat="1" ht="23.1" customHeight="1">
-      <c r="B34" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C34" s="14"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="22"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="17"/>
-    </row>
-    <row r="35" spans="2:8" s="12" customFormat="1" ht="23.1" customHeight="1">
-      <c r="C35" s="27"/>
-      <c r="E35" s="28"/>
-      <c r="G35" s="29"/>
-    </row>
-    <row r="36" spans="2:8" s="12" customFormat="1" ht="23.1" customHeight="1">
-      <c r="C36" s="27"/>
-      <c r="E36" s="28"/>
-      <c r="G36" s="29"/>
-    </row>
-    <row r="37" spans="2:8" s="12" customFormat="1" ht="23.1" customHeight="1">
-      <c r="C37" s="27"/>
-      <c r="E37" s="28"/>
-      <c r="G37" s="29"/>
-    </row>
-    <row r="38" spans="2:8" s="12" customFormat="1" ht="23.1" customHeight="1">
-      <c r="C38" s="27"/>
-      <c r="E38" s="28"/>
-      <c r="G38" s="29"/>
-    </row>
-    <row r="39" spans="2:8" s="12" customFormat="1" ht="23.1" customHeight="1">
-      <c r="C39" s="27"/>
-      <c r="E39" s="28"/>
-      <c r="G39" s="29"/>
-    </row>
-    <row r="40" spans="2:8" s="12" customFormat="1" ht="23.1" customHeight="1">
-      <c r="C40" s="27"/>
-      <c r="E40" s="28"/>
-      <c r="G40" s="29"/>
-    </row>
-    <row r="41" spans="2:8" s="12" customFormat="1" ht="23.1" customHeight="1">
-      <c r="C41" s="27"/>
-      <c r="E41" s="28"/>
-      <c r="G41" s="29"/>
-    </row>
-    <row r="42" spans="2:8" s="12" customFormat="1" ht="23.1" customHeight="1">
-      <c r="C42" s="27"/>
-      <c r="E42" s="28"/>
-      <c r="G42" s="29"/>
-    </row>
-    <row r="43" spans="2:8" s="12" customFormat="1" ht="23.1" customHeight="1">
-      <c r="C43" s="27"/>
-      <c r="E43" s="28"/>
-      <c r="G43" s="29"/>
-    </row>
-    <row r="44" spans="2:8" s="12" customFormat="1" ht="23.1" customHeight="1">
-      <c r="C44" s="27"/>
-      <c r="E44" s="28"/>
-      <c r="G44" s="29"/>
-    </row>
-    <row r="45" spans="2:8" s="12" customFormat="1" ht="23.1" customHeight="1">
-      <c r="C45" s="27"/>
-      <c r="E45" s="28"/>
-      <c r="G45" s="29"/>
-    </row>
-    <row r="46" spans="2:8" s="12" customFormat="1" ht="23.1" customHeight="1">
-      <c r="C46" s="27"/>
-      <c r="E46" s="28"/>
-      <c r="G46" s="29"/>
-    </row>
-    <row r="47" spans="2:8" s="12" customFormat="1" ht="23.1" customHeight="1">
-      <c r="C47" s="27"/>
-      <c r="E47" s="28"/>
-      <c r="G47" s="29"/>
-    </row>
-    <row r="48" spans="2:8" s="12" customFormat="1" ht="23.1" customHeight="1">
-      <c r="C48" s="27"/>
-      <c r="E48" s="28"/>
-      <c r="G48" s="29"/>
-    </row>
-    <row r="49" spans="3:7" s="12" customFormat="1" ht="23.1" customHeight="1">
-      <c r="C49" s="27"/>
-      <c r="E49" s="28"/>
-      <c r="G49" s="29"/>
-    </row>
-    <row r="50" spans="3:7" s="12" customFormat="1" ht="23.1" customHeight="1">
-      <c r="C50" s="27"/>
-      <c r="E50" s="28"/>
-      <c r="G50" s="29"/>
-    </row>
-    <row r="51" spans="3:7" s="12" customFormat="1" ht="23.1" customHeight="1">
-      <c r="C51" s="27"/>
-      <c r="E51" s="28"/>
-      <c r="G51" s="29"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" s="11" customFormat="1" ht="33" customHeight="1" thickBot="1">
+      <c r="B14" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14" s="21"/>
+      <c r="F14" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+    </row>
+    <row r="15" spans="2:11" s="11" customFormat="1" ht="30.75" thickBot="1">
+      <c r="B15" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" s="21"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" s="16"/>
+    </row>
+    <row r="16" spans="2:11" s="11" customFormat="1" ht="15.75" thickBot="1">
+      <c r="B16" s="12"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+    </row>
+    <row r="17" spans="2:8" s="11" customFormat="1" ht="23.1" customHeight="1">
+      <c r="B17" s="12"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+    </row>
+    <row r="18" spans="2:8" s="11" customFormat="1" ht="23.1" customHeight="1">
+      <c r="B18" s="12"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+    </row>
+    <row r="19" spans="2:8" s="11" customFormat="1" ht="23.1" customHeight="1">
+      <c r="B19" s="12"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+    </row>
+    <row r="20" spans="2:8" s="11" customFormat="1" ht="23.1" customHeight="1">
+      <c r="B20" s="12"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+    </row>
+    <row r="21" spans="2:8" s="11" customFormat="1" ht="23.1" customHeight="1">
+      <c r="B21" s="12"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+    </row>
+    <row r="22" spans="2:8" s="11" customFormat="1" ht="23.1" customHeight="1">
+      <c r="B22" s="12"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+    </row>
+    <row r="23" spans="2:8" s="11" customFormat="1" ht="23.1" customHeight="1">
+      <c r="B23" s="12"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+    </row>
+    <row r="24" spans="2:8" s="11" customFormat="1" ht="23.1" customHeight="1">
+      <c r="B24" s="12"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+    </row>
+    <row r="25" spans="2:8" s="11" customFormat="1" ht="23.1" customHeight="1">
+      <c r="B25" s="12"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
+    </row>
+    <row r="26" spans="2:8" s="11" customFormat="1" ht="23.1" customHeight="1">
+      <c r="B26" s="12"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
+    </row>
+    <row r="27" spans="2:8" s="11" customFormat="1" ht="23.1" customHeight="1">
+      <c r="B27" s="12"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="16"/>
+    </row>
+    <row r="28" spans="2:8" s="11" customFormat="1" ht="23.1" customHeight="1">
+      <c r="B28" s="12"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="16"/>
+    </row>
+    <row r="29" spans="2:8" s="11" customFormat="1" ht="23.1" customHeight="1">
+      <c r="B29" s="12"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
+    </row>
+    <row r="30" spans="2:8" s="11" customFormat="1" ht="23.1" customHeight="1">
+      <c r="B30" s="12"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="16"/>
+    </row>
+    <row r="31" spans="2:8" s="11" customFormat="1" ht="23.1" customHeight="1">
+      <c r="B31" s="12"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="16"/>
+    </row>
+    <row r="32" spans="2:8" s="11" customFormat="1" ht="23.1" customHeight="1">
+      <c r="B32" s="12"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="16"/>
+      <c r="H32" s="16"/>
+    </row>
+    <row r="33" spans="2:8" s="11" customFormat="1" ht="23.1" customHeight="1">
+      <c r="B33" s="12"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="16"/>
+    </row>
+    <row r="34" spans="2:8" s="11" customFormat="1" ht="23.1" customHeight="1">
+      <c r="B34" s="12"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="16"/>
+    </row>
+    <row r="35" spans="2:8" s="11" customFormat="1" ht="23.1" customHeight="1">
+      <c r="C35" s="26"/>
+      <c r="E35" s="27"/>
+      <c r="G35" s="28"/>
+    </row>
+    <row r="36" spans="2:8" s="11" customFormat="1" ht="23.1" customHeight="1">
+      <c r="C36" s="26"/>
+      <c r="E36" s="27"/>
+      <c r="G36" s="28"/>
+    </row>
+    <row r="37" spans="2:8" s="11" customFormat="1" ht="23.1" customHeight="1">
+      <c r="C37" s="26"/>
+      <c r="E37" s="27"/>
+      <c r="G37" s="28"/>
+    </row>
+    <row r="38" spans="2:8" s="11" customFormat="1" ht="23.1" customHeight="1">
+      <c r="C38" s="26"/>
+      <c r="E38" s="27"/>
+      <c r="G38" s="28"/>
+    </row>
+    <row r="39" spans="2:8" s="11" customFormat="1" ht="23.1" customHeight="1">
+      <c r="C39" s="26"/>
+      <c r="E39" s="27"/>
+      <c r="G39" s="28"/>
+    </row>
+    <row r="40" spans="2:8" s="11" customFormat="1" ht="23.1" customHeight="1">
+      <c r="C40" s="26"/>
+      <c r="E40" s="27"/>
+      <c r="G40" s="28"/>
+    </row>
+    <row r="41" spans="2:8" s="11" customFormat="1" ht="23.1" customHeight="1">
+      <c r="C41" s="26"/>
+      <c r="E41" s="27"/>
+      <c r="G41" s="28"/>
+    </row>
+    <row r="42" spans="2:8" s="11" customFormat="1" ht="23.1" customHeight="1">
+      <c r="C42" s="26"/>
+      <c r="E42" s="27"/>
+      <c r="G42" s="28"/>
+    </row>
+    <row r="43" spans="2:8" s="11" customFormat="1" ht="23.1" customHeight="1">
+      <c r="C43" s="26"/>
+      <c r="E43" s="27"/>
+      <c r="G43" s="28"/>
+    </row>
+    <row r="44" spans="2:8" s="11" customFormat="1" ht="23.1" customHeight="1">
+      <c r="C44" s="26"/>
+      <c r="E44" s="27"/>
+      <c r="G44" s="28"/>
+    </row>
+    <row r="45" spans="2:8" s="11" customFormat="1" ht="23.1" customHeight="1">
+      <c r="C45" s="26"/>
+      <c r="E45" s="27"/>
+      <c r="G45" s="28"/>
+    </row>
+    <row r="46" spans="2:8" s="11" customFormat="1" ht="23.1" customHeight="1">
+      <c r="C46" s="26"/>
+      <c r="E46" s="27"/>
+      <c r="G46" s="28"/>
+    </row>
+    <row r="47" spans="2:8" s="11" customFormat="1" ht="23.1" customHeight="1">
+      <c r="C47" s="26"/>
+      <c r="E47" s="27"/>
+      <c r="G47" s="28"/>
+    </row>
+    <row r="48" spans="2:8" s="11" customFormat="1" ht="23.1" customHeight="1">
+      <c r="C48" s="26"/>
+      <c r="E48" s="27"/>
+      <c r="G48" s="28"/>
+    </row>
+    <row r="49" spans="3:7" s="11" customFormat="1" ht="23.1" customHeight="1">
+      <c r="C49" s="26"/>
+      <c r="E49" s="27"/>
+      <c r="G49" s="28"/>
+    </row>
+    <row r="50" spans="3:7" s="11" customFormat="1" ht="23.1" customHeight="1">
+      <c r="C50" s="26"/>
+      <c r="E50" s="27"/>
+      <c r="G50" s="28"/>
+    </row>
+    <row r="51" spans="3:7" s="11" customFormat="1" ht="23.1" customHeight="1">
+      <c r="C51" s="26"/>
+      <c r="E51" s="27"/>
+      <c r="G51" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:H2"/>
   </mergeCells>
   <conditionalFormatting sqref="B5:E5 E6 C5:C6 B6:B34">
-    <cfRule type="expression" dxfId="20" priority="2">
+    <cfRule type="expression" dxfId="29" priority="11">
       <formula>$B5="Done!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="3">
+    <cfRule type="expression" dxfId="28" priority="12">
       <formula>$B5="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="4">
+    <cfRule type="expression" dxfId="27" priority="13">
       <formula>$B5="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="5">
+    <cfRule type="expression" dxfId="26" priority="14">
       <formula>$B5="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="expression" dxfId="16" priority="6">
+    <cfRule type="expression" dxfId="25" priority="15">
       <formula>$B7="Done!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="7">
+    <cfRule type="expression" dxfId="24" priority="16">
       <formula>$B7="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="8">
+    <cfRule type="expression" dxfId="23" priority="17">
       <formula>$B7="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="9">
+    <cfRule type="expression" dxfId="22" priority="18">
       <formula>$B7="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="expression" dxfId="12" priority="10">
+    <cfRule type="expression" dxfId="21" priority="19">
       <formula>$B6="Done!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="11">
+    <cfRule type="expression" dxfId="20" priority="20">
       <formula>$B6="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="12">
+    <cfRule type="expression" dxfId="19" priority="21">
       <formula>$B6="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="13">
+    <cfRule type="expression" dxfId="18" priority="22">
       <formula>$B6="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C7:C34">
-    <cfRule type="expression" dxfId="8" priority="14">
+  <conditionalFormatting sqref="C7:C14 C16:C34">
+    <cfRule type="expression" dxfId="17" priority="23">
       <formula>$B7="Done!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="15">
+    <cfRule type="expression" dxfId="16" priority="24">
       <formula>$B7="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="16">
+    <cfRule type="expression" dxfId="15" priority="25">
       <formula>$B7="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="17">
+    <cfRule type="expression" dxfId="14" priority="26">
       <formula>$B7="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D8:D34">
-    <cfRule type="expression" dxfId="4" priority="18">
+  <conditionalFormatting sqref="D8:D14 D16:D34">
+    <cfRule type="expression" dxfId="13" priority="27">
       <formula>$B$4="Plannedd"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="19">
+    <cfRule type="expression" dxfId="12" priority="28">
       <formula>$B8="Done!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="20">
+    <cfRule type="expression" dxfId="11" priority="29">
       <formula>$B8="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="21">
+    <cfRule type="expression" dxfId="10" priority="30">
       <formula>$B8="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="22">
+    <cfRule type="expression" dxfId="9" priority="31">
       <formula>$B8="Dropped"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C15">
+    <cfRule type="expression" dxfId="8" priority="1">
+      <formula>$B15="Done!"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="2">
+      <formula>$B15="Ongoing"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="3">
+      <formula>$B15="Blocked"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="4">
+      <formula>$B15="Dropped"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D15">
+    <cfRule type="expression" dxfId="4" priority="5">
+      <formula>$B$4="Plannedd"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="6">
+      <formula>$B15="Done!"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="7">
+      <formula>$B15="Ongoing"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="8">
+      <formula>$B15="Blocked"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="9">
+      <formula>$B15="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -2212,187 +2228,187 @@
   <dimension ref="A1:AMJ27"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="79.42578125" style="30" customWidth="1"/>
-    <col min="2" max="2" width="43.85546875" style="30" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" style="31" customWidth="1"/>
-    <col min="4" max="1024" width="10.85546875" style="31"/>
+    <col min="1" max="1" width="79.42578125" style="29" customWidth="1"/>
+    <col min="2" max="2" width="43.85546875" style="29" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" style="30" customWidth="1"/>
+    <col min="4" max="1024" width="10.85546875" style="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="33" customFormat="1" ht="30" customHeight="1">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:8" s="32" customFormat="1" ht="30" customHeight="1">
+      <c r="A1" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="34"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="34"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="34"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="34"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="34"/>
+      <c r="H6" s="30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="33"/>
+      <c r="B7" s="34"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="33"/>
+      <c r="B8" s="34"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="33"/>
+      <c r="B9" s="34"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="33"/>
+      <c r="B10" s="34"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="33"/>
+      <c r="B11" s="34"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="33"/>
+      <c r="B12" s="35"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="33"/>
+      <c r="B13" s="34"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="36"/>
+      <c r="C14" s="37"/>
+    </row>
+    <row r="16" spans="1:8" ht="68.25" customHeight="1">
+      <c r="A16" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="38" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="23.25">
+      <c r="A17" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="40" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="23.25">
+      <c r="A18" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="40" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="23.25">
+      <c r="A19" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="40" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="23.25">
+      <c r="A20" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="40" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="23.25">
+      <c r="A21" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="40" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="23.25">
+      <c r="A22" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="40" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="23.25">
+      <c r="A23" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="32" t="s">
+    </row>
+    <row r="24" spans="1:2" ht="23.25">
+      <c r="A24" s="39" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="34" t="s">
+      <c r="B24" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="35"/>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="34" t="s">
+    </row>
+    <row r="25" spans="1:2" ht="23.25">
+      <c r="A25" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="35"/>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="34" t="s">
+      <c r="B25" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="35"/>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="35"/>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="35"/>
-      <c r="H6" s="31" t="s">
+    </row>
+    <row r="26" spans="1:2" ht="23.25">
+      <c r="A26" s="39" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="34"/>
-      <c r="B7" s="35"/>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="34"/>
-      <c r="B8" s="35"/>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="34"/>
-      <c r="B9" s="35"/>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="34"/>
-      <c r="B10" s="35"/>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="34"/>
-      <c r="B11" s="35"/>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="34"/>
-      <c r="B12" s="36"/>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="34"/>
-      <c r="B13" s="35"/>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="37" t="s">
+      <c r="B26" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="37"/>
-      <c r="C14" s="38"/>
-    </row>
-    <row r="16" spans="1:8" ht="68.25" customHeight="1">
-      <c r="A16" s="39" t="s">
+    </row>
+    <row r="27" spans="1:2" ht="23.25">
+      <c r="A27" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="39" t="s">
+      <c r="B27" s="40" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="23.25">
-      <c r="A17" s="40" t="s">
-        <v>49</v>
-      </c>
-      <c r="B17" s="41" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="23.25">
-      <c r="A18" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="B18" s="41" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="23.25">
-      <c r="A19" s="40" t="s">
-        <v>53</v>
-      </c>
-      <c r="B19" s="41" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="23.25">
-      <c r="A20" s="40" t="s">
-        <v>55</v>
-      </c>
-      <c r="B20" s="41" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="23.25">
-      <c r="A21" s="40" t="s">
-        <v>57</v>
-      </c>
-      <c r="B21" s="41" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="23.25">
-      <c r="A22" s="40" t="s">
-        <v>59</v>
-      </c>
-      <c r="B22" s="41" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="23.25">
-      <c r="A23" s="40" t="s">
-        <v>61</v>
-      </c>
-      <c r="B23" s="41" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="23.25">
-      <c r="A24" s="40" t="s">
-        <v>63</v>
-      </c>
-      <c r="B24" s="41" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="23.25">
-      <c r="A25" s="40" t="s">
-        <v>65</v>
-      </c>
-      <c r="B25" s="41" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="23.25">
-      <c r="A26" s="40" t="s">
-        <v>67</v>
-      </c>
-      <c r="B26" s="41" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="23.25">
-      <c r="A27" s="40" t="s">
-        <v>69</v>
-      </c>
-      <c r="B27" s="41" t="s">
-        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>